<commit_message>
added tip&trick a1b*a2b (if a1+a2=10)
</commit_message>
<xml_diff>
--- a/NetApps/PrepareReportApp/CompanyInvoiceTemplate.xlsx
+++ b/NetApps/PrepareReportApp/CompanyInvoiceTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\AN_Assembla\trunk\PrepareReport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\GitHub\DiverseAN\NetApps\PrepareReportApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6175FE64-1D62-428C-A425-03F77A3C5CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF808D3C-72C0-4FFB-B96A-32981A954D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>NewGround Ltd</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>Bank account (IBAN Code):</t>
-  </si>
-  <si>
-    <t>UA183808050000000026005189407</t>
   </si>
   <si>
     <t>Bank of beneficiary:</t>
@@ -148,6 +145,12 @@
   </si>
   <si>
     <t>Old reates</t>
+  </si>
+  <si>
+    <t>UA883003350000000026005189407</t>
+  </si>
+  <si>
+    <t>NewGround LLC</t>
   </si>
 </sst>
 </file>
@@ -157,7 +160,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +194,13 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
@@ -233,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -263,6 +273,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,9 +371,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -400,9 +411,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -435,26 +446,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -487,26 +481,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -682,7 +659,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:G20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -695,15 +674,14 @@
     <col min="7" max="7" width="9.5546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.5546875" style="2" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="14" width="10.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="14" width="10.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="15" max="16384" width="10.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K1" s="1" t="str">
         <f ca="1">MID(CELL("filename"),SEARCH("[",CELL("filename"))+1, SEARCH("]",CELL("filename"))-SEARCH("[",CELL("filename"))-1)</f>
-        <v>NG.SoftwareAces.2023-01-08 Invoice 230108-01.xlsx</v>
+        <v>CompanyInvoiceTemplate.xlsx</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
@@ -715,7 +693,7 @@
       </c>
       <c r="K2" s="1" t="str">
         <f ca="1">MID(K1,17,10)</f>
-        <v>2023-01-08</v>
+        <v>mplate.xls</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
@@ -727,7 +705,7 @@
       </c>
       <c r="K3" s="1" t="str">
         <f ca="1">MID(K1,36,9)</f>
-        <v>230108-01</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
@@ -741,22 +719,22 @@
     <row r="5" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="K5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="K6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L6" s="17">
-        <v>36.5</v>
+        <v>37.049999999999997</v>
       </c>
       <c r="N6" s="1">
         <v>34.909999999999997</v>
@@ -765,10 +743,10 @@
     <row r="7" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
       <c r="I7" s="4"/>
       <c r="K7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L7" s="1">
-        <v>30.14</v>
+        <v>30.82</v>
       </c>
       <c r="N7" s="6">
         <f>23.04+0.705326087</f>
@@ -782,13 +760,13 @@
       <c r="C8" s="5"/>
       <c r="D8" s="14" t="str">
         <f ca="1">K3</f>
-        <v>230108-01</v>
+        <v/>
       </c>
       <c r="K8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L8" s="1">
-        <v>31.73</v>
+        <v>32.44</v>
       </c>
       <c r="N8" s="6">
         <f>23.04+0.705326087</f>
@@ -799,9 +777,9 @@
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="15" t="e">
         <f ca="1">DATEVALUE(K2)</f>
-        <v>44934</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
@@ -812,9 +790,15 @@
         <v>9</v>
       </c>
       <c r="L10" s="17"/>
+      <c r="N10" s="17">
+        <v>36.5</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
       <c r="H11" s="6"/>
+      <c r="N11" s="1">
+        <v>30.14</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
@@ -833,10 +817,13 @@
       <c r="H12" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="N12" s="1">
+        <v>31.73</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -892,24 +879,24 @@
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>0</v>
+      <c r="C18" s="21" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>19</v>
+      <c r="C19" s="21" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>20</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>21</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
@@ -918,41 +905,41 @@
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>